<commit_message>
da validate xong create booking ca 2 ben
</commit_message>
<xml_diff>
--- a/backend/exports/Bao-cao-doanh-thu-Thang-12-2024.xlsx
+++ b/backend/exports/Bao-cao-doanh-thu-Thang-12-2024.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="69">
   <si>
     <t>BẢNG KÊ DOANH THU</t>
   </si>
@@ -83,108 +83,111 @@
     <t>Ghi chú</t>
   </si>
   <si>
+    <t>phòng VIP</t>
+  </si>
+  <si>
+    <t>450,000</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tổng:</t>
+  </si>
+  <si>
+    <t>900,000</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu:</t>
+  </si>
+  <si>
+    <t>Số phòng:</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Số đoàn:</t>
+  </si>
+  <si>
+    <t>NGÀY 2/12/2024</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>NGÀY 3/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 4/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 5/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 6/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 7/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 8/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 9/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 10/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 11/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 12/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 13/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 14/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 15/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 16/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 17/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 18/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 19/12/2024</t>
+  </si>
+  <si>
+    <t>NGÀY 20/12/2024</t>
+  </si>
+  <si>
     <t>phòng đôi</t>
   </si>
   <si>
     <t>400,000</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>phòng VIP</t>
-  </si>
-  <si>
-    <t>450,000</t>
-  </si>
-  <si>
-    <t>Tổng:</t>
-  </si>
-  <si>
-    <t>1,300,000</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu:</t>
-  </si>
-  <si>
-    <t>Số phòng:</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>NGÀY 21/12/2024</t>
+  </si>
+  <si>
+    <t>1,250,000</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Số đoàn:</t>
-  </si>
-  <si>
-    <t>NGÀY 2/12/2024</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>NGÀY 3/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 4/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 5/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 6/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 7/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 8/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 9/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 10/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 11/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 12/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 13/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 14/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 15/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 16/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 17/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 18/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 19/12/2024</t>
-  </si>
-  <si>
-    <t>NGÀY 20/12/2024</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>NGÀY 21/12/2024</t>
-  </si>
-  <si>
-    <t>1,250,000</t>
-  </si>
-  <si>
     <t>NGÀY 22/12/2024</t>
   </si>
   <si>
@@ -195,9 +198,6 @@
   </si>
   <si>
     <t>800,000</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>NGÀY 25/12/2024</t>
@@ -652,7 +652,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -759,106 +759,79 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
+      <c r="B7" s="6">
+        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="6">
-        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -866,14 +839,6 @@
         <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -910,7 +875,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -958,7 +923,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -970,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -987,7 +952,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -995,15 +960,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1042,7 +1007,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1090,7 +1055,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1102,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1119,7 +1084,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1127,15 +1092,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1174,7 +1139,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1222,7 +1187,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1234,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1251,7 +1216,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1259,15 +1224,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1306,7 +1271,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1354,7 +1319,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1366,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1383,7 +1348,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1391,15 +1356,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1438,7 +1403,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1486,7 +1451,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1498,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1515,7 +1480,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1523,15 +1488,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1570,7 +1535,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1618,7 +1583,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1630,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1647,7 +1612,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1655,15 +1620,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1702,7 +1667,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1750,7 +1715,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1762,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1779,7 +1744,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1787,15 +1752,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1834,7 +1799,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1882,7 +1847,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -1894,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -1911,7 +1876,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -1919,15 +1884,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -1966,7 +1931,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2014,7 +1979,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2026,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -2043,7 +2008,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2051,15 +2016,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -2098,7 +2063,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2146,7 +2111,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2158,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -2175,7 +2140,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2183,15 +2148,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -2230,7 +2195,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2278,7 +2243,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2290,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -2307,7 +2272,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2315,15 +2280,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -2362,7 +2327,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2413,16 +2378,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -2445,7 +2410,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
@@ -2457,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
@@ -2474,7 +2439,7 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2482,7 +2447,7 @@
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>44</v>
@@ -2490,7 +2455,7 @@
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>15</v>
@@ -2580,16 +2545,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -2615,16 +2580,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -2650,16 +2615,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>15</v>
@@ -2682,7 +2647,7 @@
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
@@ -2711,7 +2676,7 @@
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2719,15 +2684,15 @@
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>15</v>
@@ -2766,7 +2731,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2814,7 +2779,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2826,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -2843,7 +2808,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2851,15 +2816,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -2898,7 +2863,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2946,7 +2911,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2958,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -2975,7 +2940,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -2983,15 +2948,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3030,7 +2995,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3081,16 +3046,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -3116,16 +3081,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -3148,7 +3113,7 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
@@ -3160,7 +3125,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
@@ -3177,7 +3142,7 @@
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3185,15 +3150,15 @@
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
@@ -3280,7 +3245,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3292,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3309,7 +3274,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3317,15 +3282,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3412,7 +3377,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3424,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3441,7 +3406,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3449,15 +3414,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3544,7 +3509,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3556,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3573,7 +3538,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3581,15 +3546,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3676,7 +3641,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3688,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3705,7 +3670,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3713,15 +3678,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3808,7 +3773,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3820,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3837,7 +3802,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3845,15 +3810,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -3892,7 +3857,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3940,7 +3905,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -3952,7 +3917,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -3969,7 +3934,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -3977,15 +3942,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4072,7 +4037,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4084,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4101,7 +4066,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4109,15 +4074,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4204,7 +4169,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4216,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4233,7 +4198,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4241,15 +4206,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4321,16 +4286,16 @@
         <v>65</v>
       </c>
       <c r="C4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>16100000</v>
+        <v>15700000</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>1300000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4426,7 +4391,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4474,7 +4439,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4486,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4503,7 +4468,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4511,15 +4476,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4558,7 +4523,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4606,7 +4571,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4618,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4635,7 +4600,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4643,15 +4608,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4690,7 +4655,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4738,7 +4703,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4750,7 +4715,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4767,7 +4732,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4775,15 +4740,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4822,7 +4787,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4870,7 +4835,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -4882,7 +4847,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -4899,7 +4864,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -4907,15 +4872,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -4954,7 +4919,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5002,7 +4967,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -5014,7 +4979,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -5031,7 +4996,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -5039,15 +5004,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>
@@ -5086,7 +5051,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5134,7 +5099,7 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -5146,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
@@ -5163,7 +5128,7 @@
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6">
         <f>SUM(E:E, F:F, G:G)</f>
@@ -5171,15 +5136,15 @@
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
da fix xong hoan toàn bên creat booking, listStaff
</commit_message>
<xml_diff>
--- a/backend/exports/Bao-cao-doanh-thu-Thang-12-2024.xlsx
+++ b/backend/exports/Bao-cao-doanh-thu-Thang-12-2024.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="64">
   <si>
     <t>BẢNG KÊ DOANH THU</t>
   </si>
@@ -122,6 +122,15 @@
     <t>NGÀY 8/12/2024</t>
   </si>
   <si>
+    <t>phòng đôi</t>
+  </si>
+  <si>
+    <t>400,000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>NGÀY 9/12/2024</t>
   </si>
   <si>
@@ -164,30 +173,21 @@
     <t>NGÀY 22/12/2024</t>
   </si>
   <si>
-    <t>phòng đôi</t>
-  </si>
-  <si>
-    <t>400,000</t>
-  </si>
-  <si>
     <t>phòng VIP</t>
   </si>
   <si>
     <t>450,000</t>
   </si>
   <si>
-    <t>2,900,000</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>2,500,000</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>NGÀY 23/12/2024</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>NGÀY 24/12/2024</t>
   </si>
   <si>
@@ -230,13 +230,10 @@
     <t>Tổng doanh thu</t>
   </si>
   <si>
+    <t>8/12/2024</t>
+  </si>
+  <si>
     <t>22/12/2024</t>
-  </si>
-  <si>
-    <t>23/12/2024</t>
-  </si>
-  <si>
-    <t>26/12/2024</t>
   </si>
 </sst>
 </file>
@@ -793,7 +790,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -925,7 +922,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1057,7 +1054,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1189,7 +1186,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1321,7 +1318,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1453,7 +1450,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1585,7 +1582,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1849,7 +1846,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1981,7 +1978,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2245,7 +2242,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2377,7 +2374,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2488,7 +2485,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2560,16 +2557,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>14</v>
@@ -2595,16 +2592,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>14</v>
@@ -2630,16 +2627,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>14</v>
@@ -2665,16 +2662,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>14</v>
@@ -2700,16 +2697,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>14</v>
@@ -2735,16 +2732,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>14</v>
@@ -2765,91 +2762,56 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="10" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>14</v>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="12" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <f>SUM(E:E, F:F, G:G)</f>
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2865,7 +2827,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -2886,7 +2848,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2932,91 +2894,56 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5">
+        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5">
-        <f>SUM(E:E, F:F, G:G)</f>
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3296,7 +3223,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -3363,91 +3290,56 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5">
+        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5">
-        <f>SUM(E:E, F:F, G:G)</f>
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4255,7 +4147,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -4309,16 +4201,16 @@
         <v>62</v>
       </c>
       <c r="C4" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6">
-        <v>5200000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>0</v>
+        <v>550000</v>
       </c>
       <c r="F4" s="6">
-        <v>2900000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4329,36 +4221,16 @@
         <v>63</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D5" s="6">
-        <v>550000</v>
+        <v>5200000</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>400000</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>400000</v>
+        <v>2500000</v>
       </c>
     </row>
   </sheetData>
@@ -4901,7 +4773,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="11" width="20" customWidth="1"/>
@@ -4968,56 +4840,91 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5">
-        <f>SUM(E:E, F:F, G:G)</f>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="5">
+        <f>SUM(E:E, F:F, G:G)</f>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5054,7 +4961,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>

</xml_diff>